<commit_message>
Piwik-Seitentitel: Felder farblich hervorgehoben
</commit_message>
<xml_diff>
--- a/Piwik-Analyse/Seitentitel.xlsx
+++ b/Piwik-Analyse/Seitentitel.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbauer/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbauer/Documents/redesign-ur-rz/Piwik-Analyse/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -575,6 +575,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -856,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,37 +901,37 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1173,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1215,28 +1217,28 @@
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="7"/>
@@ -1889,6 +1891,186 @@
       <c r="H46" s="8"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D8:D13">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:D20">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D27">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D34">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:D41">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F13">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:F20">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F27">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:F34">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36:F41">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:H13">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:H20">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:H27">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29:H34">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36:H41">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1898,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1938,22 +2120,22 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="15" t="s">
         <v>43</v>
       </c>
       <c r="J7" s="2"/>
@@ -2514,6 +2696,126 @@
       <c r="F75" s="8"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D8:D13">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F13">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:D20">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D26">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D34">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:D41">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:F20">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F27">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:F34">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36:F41">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>